<commit_message>
tanuló adat módosítás, új tanulü felvevés excel filenál hozzáadva. Angol nyelv elltávolítva, és egyéb kisebb javítások. Stabil
</commit_message>
<xml_diff>
--- a/WindowsFormsApp autósiskola/bin/Debug/ExcelMasolat.xlsx
+++ b/WindowsFormsApp autósiskola/bin/Debug/ExcelMasolat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23906"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csics\Downloads\test files that works with the program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AC8B2A-1620-44C3-BFF6-C506E4640CE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F52DAB-387C-4852-B29E-7262D2717B0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019.tanulók" sheetId="5" r:id="rId1"/>
@@ -18,12 +18,24 @@
     <sheet name="2021.tanulók" sheetId="4" r:id="rId3"/>
     <sheet name="2020.tanulók(1)" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
   <si>
     <t>Sorszám</t>
   </si>
@@ -124,9 +136,6 @@
     <t>U.A.</t>
   </si>
   <si>
-    <t>Budapest</t>
-  </si>
-  <si>
     <t>Rátkai Petra</t>
   </si>
   <si>
@@ -263,6 +272,54 @@
   </si>
   <si>
     <t>megjegyzések</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2043. 06. 09. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019. 10. 24. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023. 10. 04. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1934. 02. 01. </t>
+  </si>
+  <si>
+    <t>Debrecen</t>
+  </si>
+  <si>
+    <t>0,0868055555555556</t>
+  </si>
+  <si>
+    <t>0,128472222222222</t>
+  </si>
+  <si>
+    <t>Galahgonya utca 10</t>
+  </si>
+  <si>
+    <t>0,0458333333333333</t>
+  </si>
+  <si>
+    <t>0,0875</t>
+  </si>
+  <si>
+    <t>0,129166666666667</t>
+  </si>
+  <si>
+    <t>fghdfg</t>
+  </si>
+  <si>
+    <t>Érdeklődő tanuló</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fdagsf gfad </t>
+  </si>
+  <si>
+    <t>_x000D_
+sfdghg_x000D_
+fdgj_x000D_
+gh</t>
   </si>
 </sst>
 </file>
@@ -774,13 +831,16 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - 1. jelölőszín" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1137,15 +1197,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0107E1-31F7-4C33-AA12-48414F206857}">
-  <dimension ref="A1:AH1"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1153,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1241,6 +1301,17 @@
       </c>
       <c r="AH1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1250,13 +1321,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI21"/>
+  <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AI2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1264,7 +1335,7 @@
     <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1343,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1362,10 +1433,10 @@
         <v>30</v>
       </c>
       <c r="AI1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1376,79 +1447,79 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="1">
-        <v>52391</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
         <v>32</v>
       </c>
       <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P2" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="1">
-        <v>43762</v>
-      </c>
-      <c r="P2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" t="s">
-        <v>55</v>
-      </c>
-      <c r="S2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="1">
-        <v>45203</v>
+      <c r="T2" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="U2">
         <v>4325345</v>
       </c>
       <c r="V2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="X2" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="2">
-        <v>12451</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
         <v>44</v>
       </c>
-      <c r="Z2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>45</v>
-      </c>
       <c r="AB2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC2" t="s">
         <v>27</v>
@@ -1468,52 +1539,52 @@
       <c r="AH2">
         <v>33</v>
       </c>
-      <c r="AI2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1">
         <v>28775</v>
       </c>
       <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
         <v>59</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>60</v>
       </c>
       <c r="I3" t="s">
         <v>32</v>
       </c>
       <c r="J3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
         <v>62</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" t="s">
-        <v>63</v>
       </c>
       <c r="O3" s="1">
         <v>32134</v>
@@ -1522,13 +1593,13 @@
         <v>36497</v>
       </c>
       <c r="Q3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" t="s">
         <v>64</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>65</v>
-      </c>
-      <c r="S3" t="s">
-        <v>66</v>
       </c>
       <c r="T3" s="1">
         <v>36642</v>
@@ -1579,12 +1650,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3">
         <v>8.5416666666666655E-2</v>
@@ -1686,12 +1757,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3">
         <v>8.6111111111111124E-2</v>
@@ -1793,18 +1864,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="3">
-        <v>8.6805555555555566E-2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.12847222222222224</v>
+        <v>48</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1818,8 +1889,8 @@
       <c r="H6">
         <v>7</v>
       </c>
-      <c r="I6">
-        <v>8</v>
+      <c r="I6" t="s">
+        <v>86</v>
       </c>
       <c r="J6">
         <v>9</v>
@@ -1900,18 +1971,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <v>4.5833333333333337E-2</v>
-      </c>
-      <c r="C7" s="3">
-        <v>8.7500000000000008E-2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.12916666666666668</v>
+      <c r="B7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -2003,11 +2074,11 @@
       <c r="AH7">
         <v>33</v>
       </c>
-      <c r="AI7">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2114,7 +2185,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2221,7 +2292,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2328,7 +2399,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2435,7 +2506,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2542,7 +2613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2649,7 +2720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2756,7 +2827,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2863,7 +2934,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2970,7 +3041,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3077,7 +3148,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3184,7 +3255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3291,7 +3362,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3398,12 +3469,119 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+      <c r="K22">
+        <v>11</v>
+      </c>
+      <c r="L22">
+        <v>12</v>
+      </c>
+      <c r="M22">
+        <v>13</v>
+      </c>
+      <c r="N22">
+        <v>14</v>
+      </c>
+      <c r="O22">
+        <v>15</v>
+      </c>
+      <c r="P22">
+        <v>16</v>
+      </c>
+      <c r="Q22">
+        <v>17</v>
+      </c>
+      <c r="R22">
+        <v>18</v>
+      </c>
+      <c r="S22">
+        <v>19</v>
+      </c>
+      <c r="T22">
+        <v>20</v>
+      </c>
+      <c r="U22">
+        <v>21</v>
+      </c>
+      <c r="V22">
+        <v>22</v>
+      </c>
+      <c r="W22">
+        <v>23</v>
+      </c>
+      <c r="X22">
+        <v>24</v>
+      </c>
+      <c r="Y22">
+        <v>25</v>
+      </c>
+      <c r="Z22">
+        <v>26</v>
+      </c>
+      <c r="AA22">
+        <v>27</v>
+      </c>
+      <c r="AB22">
+        <v>28</v>
+      </c>
+      <c r="AC22">
+        <v>29</v>
+      </c>
+      <c r="AD22">
+        <v>30</v>
+      </c>
+      <c r="AE22">
+        <v>31</v>
+      </c>
+      <c r="AF22">
+        <v>32</v>
+      </c>
+      <c r="AG22">
+        <v>33</v>
+      </c>
+      <c r="AH22">
+        <v>34</v>
+      </c>
+      <c r="AI22">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3417,15 +3595,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEC89F5-FB12-409E-B346-C91637EE22B2}">
-  <dimension ref="A1:AH1"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AI1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3433,7 +3611,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3521,6 +3699,150 @@
       </c>
       <c r="AH1" t="s">
         <v>30</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>'2020. tanulók (1,2)'!A2</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>'2020. tanulók (1,2)'!B2</f>
+        <v>Pál Zalán</v>
+      </c>
+      <c r="C2" t="str">
+        <f>'2020. tanulók (1,2)'!C2</f>
+        <v>U.A.</v>
+      </c>
+      <c r="D2" t="str">
+        <f>'2020. tanulók (1,2)'!D2</f>
+        <v>Debrecen</v>
+      </c>
+      <c r="E2" t="str">
+        <f>'2020. tanulók (1,2)'!E2</f>
+        <v xml:space="preserve">2043. 06. 09. </v>
+      </c>
+      <c r="F2" t="str">
+        <f>'2020. tanulók (1,2)'!F2</f>
+        <v>Rátkai Petra</v>
+      </c>
+      <c r="G2" t="str">
+        <f>'2020. tanulók (1,2)'!G2</f>
+        <v>magyar</v>
+      </c>
+      <c r="H2" t="str">
+        <f>'2020. tanulók (1,2)'!H2</f>
+        <v>9456 Narnia Hentes utca 6.</v>
+      </c>
+      <c r="I2" t="str">
+        <f>'2020. tanulók (1,2)'!I2</f>
+        <v>U.A.</v>
+      </c>
+      <c r="J2" t="str">
+        <f>'2020. tanulók (1,2)'!J2</f>
+        <v>324/432768</v>
+      </c>
+      <c r="K2" t="str">
+        <f>'2020. tanulók (1,2)'!K2</f>
+        <v>zalán2020@hangya.hu</v>
+      </c>
+      <c r="L2" t="str">
+        <f>'2020. tanulók (1,2)'!L2</f>
+        <v>x</v>
+      </c>
+      <c r="M2" t="str">
+        <f>'2020. tanulók (1,2)'!M2</f>
+        <v>új</v>
+      </c>
+      <c r="N2" t="str">
+        <f>'2020. tanulók (1,2)'!N2</f>
+        <v>213432HG/2021.06.07</v>
+      </c>
+      <c r="O2" t="str">
+        <f>'2020. tanulók (1,2)'!O2</f>
+        <v xml:space="preserve">2019. 10. 24. </v>
+      </c>
+      <c r="P2" t="str">
+        <f>'2020. tanulók (1,2)'!P2</f>
+        <v>2020.45.3</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>'2020. tanulók (1,2)'!Q2</f>
+        <v>9341/19/1008/8765</v>
+      </c>
+      <c r="R2" t="str">
+        <f>'2020. tanulók (1,2)'!R2</f>
+        <v>s-2020/43/1486</v>
+      </c>
+      <c r="S2" t="str">
+        <f>'2020. tanulók (1,2)'!S2</f>
+        <v>2020.20.2</v>
+      </c>
+      <c r="T2" t="str">
+        <f>'2020. tanulók (1,2)'!T2</f>
+        <v xml:space="preserve">2023. 10. 04. </v>
+      </c>
+      <c r="U2">
+        <f>'2020. tanulók (1,2)'!U2</f>
+        <v>4325345</v>
+      </c>
+      <c r="V2" t="str">
+        <f>'2020. tanulók (1,2)'!V2</f>
+        <v>2020.54.34</v>
+      </c>
+      <c r="W2" t="str">
+        <f>'2020. tanulók (1,2)'!W2</f>
+        <v xml:space="preserve">1934. 02. 01. </v>
+      </c>
+      <c r="X2" t="str">
+        <f>'2020. tanulók (1,2)'!X2</f>
+        <v>2020.32.3</v>
+      </c>
+      <c r="Y2" t="str">
+        <f>'2020. tanulók (1,2)'!Y2</f>
+        <v>2020.04.45</v>
+      </c>
+      <c r="Z2" t="str">
+        <f>'2020. tanulók (1,2)'!Z2</f>
+        <v>x</v>
+      </c>
+      <c r="AA2" t="str">
+        <f>'2020. tanulók (1,2)'!AA2</f>
+        <v>2020.4.6. M</v>
+      </c>
+      <c r="AB2" t="str">
+        <f>'2020. tanulók (1,2)'!AB2</f>
+        <v>x</v>
+      </c>
+      <c r="AC2" t="str">
+        <f>'2020. tanulók (1,2)'!AC2</f>
+        <v>végzett</v>
+      </c>
+      <c r="AD2">
+        <f>'2020. tanulók (1,2)'!AD2</f>
+        <v>29</v>
+      </c>
+      <c r="AE2">
+        <f>'2020. tanulók (1,2)'!AE2</f>
+        <v>30</v>
+      </c>
+      <c r="AF2">
+        <f>'2020. tanulók (1,2)'!AF2</f>
+        <v>31</v>
+      </c>
+      <c r="AG2">
+        <f>'2020. tanulók (1,2)'!AG2</f>
+        <v>32</v>
+      </c>
+      <c r="AH2">
+        <f>'2020. tanulók (1,2)'!AH2</f>
+        <v>33</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3532,7 +3854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC34D197-F2C4-4113-B90E-D50843FD16CD}">
   <dimension ref="A1:AI29"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1"/>
     </sheetView>
   </sheetViews>
@@ -3550,7 +3872,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3640,7 +3962,7 @@
         <v>30</v>
       </c>
       <c r="AI1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -3648,40 +3970,40 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>70</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>71</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>72</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>73</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
         <v>75</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" t="s">
-        <v>76</v>
       </c>
       <c r="O2" s="1">
         <v>45631</v>
@@ -3690,10 +4012,10 @@
         <v>45920</v>
       </c>
       <c r="Q2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2" t="s">
         <v>77</v>
-      </c>
-      <c r="R2" t="s">
-        <v>78</v>
       </c>
       <c r="S2" s="1">
         <v>45639</v>
@@ -3710,7 +4032,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -3718,7 +4040,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">

</xml_diff>